<commit_message>
fix: correctly escape/unescape in strings.xml and Excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/expected.xlsx
+++ b/src/test/resources/expected.xlsx
@@ -27,8 +27,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -39,8 +39,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -51,8 +51,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -63,8 +63,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -75,8 +75,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -87,8 +87,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -99,8 +99,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -111,8 +111,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -123,8 +123,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -135,8 +135,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -147,8 +147,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -159,8 +159,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -171,8 +171,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -183,8 +183,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -195,8 +195,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -207,8 +207,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -219,8 +219,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -231,8 +231,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -243,8 +243,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -255,8 +255,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -267,8 +267,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -279,8 +279,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -291,8 +291,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -303,8 +303,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -315,8 +315,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -327,8 +327,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -339,8 +339,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -351,8 +351,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -363,8 +363,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -375,8 +375,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -387,8 +387,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -399,8 +399,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -411,8 +411,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -423,8 +423,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -435,8 +435,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -447,8 +447,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -459,8 +459,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -471,8 +471,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -483,8 +483,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -495,8 +495,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -507,8 +507,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -519,8 +519,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -531,8 +531,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -543,8 +543,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -555,8 +555,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -567,8 +567,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -579,8 +579,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -591,8 +591,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -603,8 +603,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -615,8 +615,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -627,8 +627,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -639,8 +639,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -651,8 +651,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -663,8 +663,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -675,8 +675,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -687,8 +687,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -699,8 +699,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -711,8 +711,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -723,8 +723,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -735,8 +735,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -747,8 +747,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -759,8 +759,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -771,8 +771,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -783,8 +783,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -795,8 +795,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -807,8 +807,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -819,8 +819,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -831,8 +831,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -843,8 +843,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -855,8 +855,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -867,8 +867,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -879,8 +879,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -891,8 +891,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -903,8 +903,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -915,8 +915,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -927,8 +927,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -939,8 +939,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -951,8 +951,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -963,8 +963,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -975,8 +975,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -987,8 +987,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -999,8 +999,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1011,8 +1011,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1023,8 +1023,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1035,8 +1035,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1047,8 +1047,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1059,8 +1059,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1071,8 +1071,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1083,8 +1083,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1095,8 +1095,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1107,8 +1107,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1119,8 +1119,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1131,8 +1131,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1143,8 +1143,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1155,8 +1155,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1167,8 +1167,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1179,8 +1179,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1191,8 +1191,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1203,8 +1203,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1215,8 +1215,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1227,8 +1227,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1239,8 +1239,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1251,8 +1251,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1263,8 +1263,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1275,8 +1275,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1287,8 +1287,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1299,8 +1299,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1311,8 +1311,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1323,8 +1323,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1335,8 +1335,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1347,8 +1347,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1359,8 +1359,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1371,8 +1371,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1383,8 +1383,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1395,8 +1395,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1407,8 +1407,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1419,8 +1419,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1431,8 +1431,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1443,8 +1443,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1455,8 +1455,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1467,8 +1467,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1479,8 +1479,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1491,8 +1491,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1503,8 +1503,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1515,8 +1515,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1527,8 +1527,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1539,8 +1539,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1551,8 +1551,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1563,8 +1563,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1575,8 +1575,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1587,8 +1587,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1599,8 +1599,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1611,8 +1611,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1623,8 +1623,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1635,8 +1635,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1647,8 +1647,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1659,8 +1659,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1671,8 +1671,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1683,8 +1683,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1695,8 +1695,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1707,8 +1707,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1719,8 +1719,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1731,8 +1731,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1743,8 +1743,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1755,8 +1755,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1767,8 +1767,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1779,8 +1779,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1791,8 +1791,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1803,8 +1803,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1815,8 +1815,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1827,8 +1827,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1839,8 +1839,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1851,8 +1851,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1863,8 +1863,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1875,8 +1875,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1887,8 +1887,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1899,8 +1899,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1911,8 +1911,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1923,8 +1923,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1935,8 +1935,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1947,8 +1947,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1959,8 +1959,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1971,8 +1971,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1983,8 +1983,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -1995,8 +1995,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2007,8 +2007,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2019,8 +2019,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2031,8 +2031,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2043,8 +2043,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2055,8 +2055,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2067,8 +2067,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2079,8 +2079,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2091,8 +2091,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2103,8 +2103,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2115,8 +2115,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2127,8 +2127,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2139,8 +2139,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2151,8 +2151,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2163,8 +2163,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2175,8 +2175,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2187,8 +2187,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2199,8 +2199,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2211,8 +2211,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2223,8 +2223,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2235,8 +2235,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2247,8 +2247,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2259,8 +2259,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2271,8 +2271,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2283,8 +2283,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2295,8 +2295,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2307,8 +2307,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2319,8 +2319,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2331,8 +2331,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2343,8 +2343,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2355,8 +2355,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2367,8 +2367,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2379,8 +2379,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2391,8 +2391,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2403,8 +2403,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2415,8 +2415,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2427,8 +2427,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2439,8 +2439,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2451,8 +2451,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2463,8 +2463,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2475,8 +2475,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2487,8 +2487,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2499,8 +2499,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2511,8 +2511,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2523,8 +2523,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2535,8 +2535,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2547,8 +2547,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2559,8 +2559,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2571,8 +2571,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2583,8 +2583,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2595,8 +2595,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2607,8 +2607,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2619,8 +2619,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2631,8 +2631,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2643,8 +2643,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2655,8 +2655,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2667,8 +2667,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2679,8 +2679,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2691,8 +2691,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2703,8 +2703,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2715,8 +2715,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2727,8 +2727,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2739,8 +2739,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2751,8 +2751,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2763,8 +2763,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2775,8 +2775,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2787,8 +2787,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2799,8 +2799,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2811,8 +2811,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2823,8 +2823,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2835,8 +2835,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2847,8 +2847,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2859,8 +2859,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2871,8 +2871,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2883,8 +2883,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2895,8 +2895,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2907,8 +2907,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2919,8 +2919,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2931,8 +2931,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2943,8 +2943,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2955,8 +2955,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2967,8 +2967,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2979,8 +2979,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -2991,8 +2991,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3003,8 +3003,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3015,8 +3015,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3027,8 +3027,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3039,8 +3039,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3051,8 +3051,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3063,8 +3063,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3075,8 +3075,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3087,8 +3087,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3099,8 +3099,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3111,8 +3111,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3123,8 +3123,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3135,8 +3135,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3147,8 +3147,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'few'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'few'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3159,8 +3159,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3171,8 +3171,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3183,8 +3183,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3195,8 +3195,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3207,8 +3207,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3219,8 +3219,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3231,8 +3231,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3243,8 +3243,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3255,8 +3255,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'many'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'many'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3267,8 +3267,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3279,8 +3279,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3291,8 +3291,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3303,8 +3303,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3315,8 +3315,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3327,8 +3327,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3339,8 +3339,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3351,8 +3351,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3363,8 +3363,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'two'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'two'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3375,8 +3375,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3387,8 +3387,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3399,8 +3399,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3411,8 +3411,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3423,8 +3423,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3435,8 +3435,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3447,8 +3447,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3459,8 +3459,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3471,8 +3471,8 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>There is no translation needed in the default language for the quantity 'zero'.
-If this language needs a different translation for this quantity add it, otherwise ignore this row.</t>
+          <t>The default language does not need/have a translation for the quantity 'zero'.
+If this language needs a different translation for this quantity, add it, otherwise ignore this row.</t>
         </r>
       </text>
     </comment>
@@ -3483,7 +3483,7 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>This text is marked as not-translatable, do not add translations in this row.</t>
+          <t>This key is marked as not-translatable, do not add translations in this row.</t>
         </r>
       </text>
     </comment>
@@ -3494,7 +3494,7 @@
             <sz val="12.0"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>This text is marked as not-translatable, do not add translations in this row.</t>
+          <t>This key is marked as not-translatable, do not add translations in this row.</t>
         </r>
       </text>
     </comment>
@@ -3538,7 +3538,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>About</t>
+    <t>About %1$s! .🎄 &lt;b&gt;Android&lt;/b&gt; .🤣</t>
   </si>
   <si>
     <t>Über</t>
@@ -7954,7 +7954,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="298">
+  <fonts count="297">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -7986,10 +7986,6 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -9161,32 +9157,32 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="FFFFCCCC"/>
+        <fgColor indexed="29"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
+        <fgColor indexed="29"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor indexed="26"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor indexed="26"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="FFD3D3D3"/>
+        <fgColor indexed="22"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD3D3D3"/>
+        <fgColor indexed="22"/>
       </patternFill>
     </fill>
   </fills>
@@ -9220,7 +9216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyBorder="true">
       <alignment wrapText="true"/>
@@ -9237,7 +9233,6 @@
     <xf numFmtId="49" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="true" applyNumberFormat="true" applyBorder="true" applyFill="true">
       <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -9257,7 +9252,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="50"/>
   <cols>
-    <col min="1" max="1" width="30.0" customWidth="true"/>
+    <col min="1" max="1" width="40.0" customWidth="true"/>
     <col min="2" max="2" hidden="true" width="50.0" customWidth="false"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
feat: correctly un-/escape all special characters
</commit_message>
<xml_diff>
--- a/src/test/resources/expected.xlsx
+++ b/src/test/resources/expected.xlsx
@@ -3538,7 +3538,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>About %1$s! .🎄 &lt;b&gt;Android&lt;/b&gt; .🤣</t>
+    <t>About %1$s! .🎄 &lt;b&gt;Android&lt;/b&gt; .🤣 " @ ? 	 ' ©</t>
   </si>
   <si>
     <t>Über</t>
@@ -3946,7 +3946,7 @@
     <t>App per Biometrie/PIN sperren</t>
   </si>
   <si>
-    <t>Verrouiller l\'application avec la biométrie ou le code PIN de l\'appareil</t>
+    <t>Verrouiller l'application avec la biométrie ou le code PIN de l'appareil</t>
   </si>
   <si>
     <t>Usa l’accesso biometrico del dispositivo o il PIN per bloccare l’app</t>
@@ -3979,7 +3979,7 @@
     <t>Fehler bei Authentifizierung per Biometrie/PIN</t>
   </si>
   <si>
-    <t>Échec de l\'authentification biométrique/code PIN</t>
+    <t>Échec de l'authentification biométrique/code PIN</t>
   </si>
   <si>
     <t>Sblocco Biometrico/PIN non riuscito</t>
@@ -3994,7 +3994,7 @@
     <t>Dein Geräte verfügt über keine biometrischen Features</t>
   </si>
   <si>
-    <t>Aucune fonction biométrique n\'est disponible sur cet appareil</t>
+    <t>Aucune fonction biométrique n'est disponible sur cet appareil</t>
   </si>
   <si>
     <t>Biometria non disponibile su questo dispositivo</t>
@@ -4009,7 +4009,7 @@
     <t>Biometrie/PIN wurde für dein Gerät noch nicht eingerichtet</t>
   </si>
   <si>
-    <t>Aucun verrouillage biométrique/code PIN n\'est paramétré sur cet appareil</t>
+    <t>Aucun verrouillage biométrique/code PIN n'est paramétré sur cet appareil</t>
   </si>
   <si>
     <t>Biometria/PIN non sono ancora configurati sul tuo dispositivo</t>
@@ -4105,7 +4105,7 @@
     <t>Can’t add %d file</t>
   </si>
   <si>
-    <t>%d fichier n\'a pas pu être ajouté</t>
+    <t>%d fichier n'a pas pu être ajouté</t>
   </si>
   <si>
     <t>Impossibile aggiungere %d file</t>
@@ -4117,7 +4117,7 @@
     <t>Can’t add %d files</t>
   </si>
   <si>
-    <t>%d fichiers n\'ont pas pu être ajoutés</t>
+    <t>%d fichiers n'ont pas pu être ajoutés</t>
   </si>
   <si>
     <t>cant_add_files_PLURALS_two</t>
@@ -4141,7 +4141,7 @@
     <t>Kann %d Bild nicht hinzufügen</t>
   </si>
   <si>
-    <t>Impossible d\'ajouter %d image</t>
+    <t>Impossible d'ajouter %d image</t>
   </si>
   <si>
     <t>Impossibile aggiungere %d immagine</t>
@@ -4156,7 +4156,7 @@
     <t>Kann %d Bilder nicht hinzufügen</t>
   </si>
   <si>
-    <t>Impossible d\'ajouter %d images</t>
+    <t>Impossible d'ajouter %d images</t>
   </si>
   <si>
     <t>Impossibile aggiungere %d immagini</t>
@@ -4228,7 +4228,7 @@
     <t>Bild kann nicht geladen werden. Es kann verschoben oder gelöscht worden sein</t>
   </si>
   <si>
-    <t>Impossible de charger l\'image. Elle a peut-être été déplacée ou supprimée.</t>
+    <t>Impossible de charger l'image. Elle a peut-être été déplacée ou supprimée.</t>
   </si>
   <si>
     <t>Impossibile caricare l’immagine. Potrebbe essere stata spostata o cancellata</t>
@@ -4375,7 +4375,7 @@
     <t>Wähle von welcher App importiert werden soll</t>
   </si>
   <si>
-    <t>Choisissez l\'application depuis laquelle importer</t>
+    <t>Choisissez l'application depuis laquelle importer</t>
   </si>
   <si>
     <t>Scegli da quale app importare</t>
@@ -4489,7 +4489,7 @@
     <t>Densidad de contenido</t>
   </si>
   <si>
-    <t>Densité d\'affichage</t>
+    <t>Densité d'affichage</t>
   </si>
   <si>
     <t>Densità del contenuto</t>
@@ -4579,7 +4579,7 @@
     <t>No hay etiquetas. ¿Crear una?</t>
   </si>
   <si>
-    <t>Il n\'existe pas encore d\'étiquettes. En créer une ?</t>
+    <t>Il n'existe pas encore d'étiquettes. En créer une ?</t>
   </si>
   <si>
     <t>Non ci sono etichette. Vuoi crearne una?</t>
@@ -4783,7 +4783,7 @@
     <t>Aufnahme für immer löschen?</t>
   </si>
   <si>
-    <t>Supprimer définitivement l\'enregistrement ?</t>
+    <t>Supprimer définitivement l'enregistrement ?</t>
   </si>
   <si>
     <t>Eliminare la registrazione audio definitivamente?</t>
@@ -4810,13 +4810,13 @@
     <t>delete_file</t>
   </si>
   <si>
-    <t>Delete file \'%s\'?</t>
-  </si>
-  <si>
-    <t>Datei \'%s\' löschen?</t>
-  </si>
-  <si>
-    <t>Supprimer le fichier \'%s\'?</t>
+    <t>Delete file '%s'?</t>
+  </si>
+  <si>
+    <t>Datei '%s' löschen?</t>
+  </si>
+  <si>
+    <t>Supprimer le fichier '%s'?</t>
   </si>
   <si>
     <t>Eliminare il file \’%s\’?</t>
@@ -4855,7 +4855,7 @@
     <t>Bild endgültig löschen?</t>
   </si>
   <si>
-    <t>Supprimer l\'image définitivement ?</t>
+    <t>Supprimer l'image définitivement ?</t>
   </si>
   <si>
     <t>Eliminare l’immagine definitivamente?</t>
@@ -4873,7 +4873,7 @@
     <t>¿Eliminar etiqueta?</t>
   </si>
   <si>
-    <t>Supprimer l\'étiquette ?</t>
+    <t>Supprimer l'étiquette ?</t>
   </si>
   <si>
     <t>Eliminare etichetta?</t>
@@ -5203,7 +5203,7 @@
     <t>Editar etiqueta</t>
   </si>
   <si>
-    <t>Modifier l\'étiquette</t>
+    <t>Modifier l'étiquette</t>
   </si>
   <si>
     <t>Modifica etichetta</t>
@@ -5350,7 +5350,7 @@
     <t>Fehler beim Umbenennen des Bildes</t>
   </si>
   <si>
-    <t>Erreur lors du renommage de l\'image</t>
+    <t>Erreur lors du renommage de l'image</t>
   </si>
   <si>
     <t>Errore durante la rinomina dell’immagine</t>
@@ -5365,16 +5365,20 @@
     <t>evernote_help</t>
   </si>
   <si>
-    <t>In order to import your Notes from Evernote you must export your Evernote Notebook as ENEX. Click Help to get more information.\n\nIf you already have a ENEX file, click Import and choose it.</t>
-  </si>
-  <si>
-    <t>Um deine Notizen von Evernote zu importierten, exportiere dein Evernote Notebook als ENEX. Klicke Hilfe für mehr Infos.\n\nFalls du schon ein ENEX Datei hast, klicke Import und wähle es aus.</t>
-  </si>
-  <si>
-    <t>Pour importer vos notes depuis Evernote, vous devez exporter votre carnet de notes Evernote au format ENEX. Cliquez sur "Aide" pour plus d\'information.\n\nSi vous possédez déjà un fichier ENEX, cliquez sur "Importer" et sélectionnez-le.</t>
-  </si>
-  <si>
-    <t>Per importare le note da Evernote devi esportare il tuo Notebook Evernote come ENEX. Clicca su Aiuto per ulteriori informazioni.\n\nSe hai già un file ENEX, clicca Importa e selezionalo.</t>
+    <t>In order to import your Notes from Evernote you must export your Evernote Notebook as ENEX. Click Help to get more information.
+If you already have a ENEX file, click Import and choose it.</t>
+  </si>
+  <si>
+    <t>Um deine Notizen von Evernote zu importierten, exportiere dein Evernote Notebook als ENEX. Klicke Hilfe für mehr Infos.
+Falls du schon ein ENEX Datei hast, klicke Import und wähle es aus.</t>
+  </si>
+  <si>
+    <t>Pour importer vos notes depuis Evernote, vous devez exporter votre carnet de notes Evernote au format ENEX. Cliquez sur "Aide" pour plus d'information.
+Si vous possédez déjà un fichier ENEX, cliquez sur "Importer" et sélectionnez-le.</t>
+  </si>
+  <si>
+    <t>Per importare le note da Evernote devi esportare il tuo Notebook Evernote come ENEX. Clicca su Aiuto per ulteriori informazioni.
+Se hai già un file ENEX, clicca Importa e selezionalo.</t>
   </si>
   <si>
     <t>export</t>
@@ -5446,19 +5450,22 @@
     <t>Import der Einstellungen fehlgeschlagen, wurde die richtige Datei ausgewählt?</t>
   </si>
   <si>
-    <t>Échec de l\'exportation des paramètres, avez-vous choisi un chemin invalide ?</t>
+    <t>Échec de l'exportation des paramètres, avez-vous choisi un chemin invalide ?</t>
   </si>
   <si>
     <t>export_settings_message</t>
   </si>
   <si>
-    <t>All Settings will be exported to a JSON file, which can be used to re-import stored settings.\n\nBe aware, that this does not include encrypted settings like the auto-backup password or the biometric encryption key</t>
-  </si>
-  <si>
-    <t>Alle Einstellungen werden als JSON Datei exportiert, die dann zum Re-Import genutzt werden kann.\n\nBeachte das hier bei verschlüsselte Einstellungen wie das Auto-Backup Passwort oder die biometrische Verschlüssung nicht exportiert wird</t>
-  </si>
-  <si>
-    <t>Tous les paramètres seront exportés dans un fichier JSON, qui pourra être utilisé pour réimporter les paramètres enregistrés.\n\nVeuillez noter que cela n\'inclut pas les paramètres chiffrés, tels que le mot de passe de sauvegarde automatique ou la clé de chiffrement biométrique.</t>
+    <t>All Settings will be exported to a JSON file, which can be used to re-import stored settings.
+Be aware, that this does not include encrypted settings like the auto-backup password or the biometric encryption key</t>
+  </si>
+  <si>
+    <t>Alle Einstellungen werden als JSON Datei exportiert, die dann zum Re-Import genutzt werden kann.
+Beachte das hier bei verschlüsselte Einstellungen wie das Auto-Backup Passwort oder die biometrische Verschlüssung nicht exportiert wird</t>
+  </si>
+  <si>
+    <t>Tous les paramètres seront exportés dans un fichier JSON, qui pourra être utilisé pour réimporter les paramètres enregistrés.
+Veuillez noter que cela n'inclut pas les paramètres chiffrés, tels que le mot de passe de sauvegarde automatique ou la clé de chiffrement biométrique.</t>
   </si>
   <si>
     <t>export_settings_success</t>
@@ -5491,16 +5498,19 @@
     <t>external_data_message</t>
   </si>
   <si>
-    <t>By enabling this, the app’s internal database will be moved into the app’s external storage (Android/media/com.philkes.notallyx).\nIn combination with file synchronization apps this can be used to synchronize NotallyX data between multiple devices.</t>
+    <t>By enabling this, the app’s internal database will be moved into the app’s external storage (Android/media/com.philkes.notallyx).
+In combination with file synchronization apps this can be used to synchronize NotallyX data between multiple devices.</t>
   </si>
   <si>
     <t>Wird dies aktiviert, wird die app-interne Datenbank in den app-externen Speicher ausgelagert (Android/media/com.philkes.notallyx). In Kombination mit Datei-Synchronisations Apps kann dies genutzt werden um NotallyX Daten zwischen mehrere Geräte zu synchronisieren.</t>
   </si>
   <si>
-    <t>En activant cette option, la base de données interne de l\'application sera déplacée vers le stockage externe de l\'application (Android/media/com.philkes.notallyx).\nEn combinaison avec des applications de synchronisation de fichiers, cela peut être utilisé pour synchroniser les données de NotallyX entre plusieurs appareils.</t>
-  </si>
-  <si>
-    <t>Attivandolo, il database interno dell’app verrà spostato nella memoria esterna dell’app (Android/media/com.philkes.notallyx).\nAbbinandolo con un’app di sincronizzazione file potrai così sincronizzare i dati di NotallyX tra dispositivi diversi.</t>
+    <t>En activant cette option, la base de données interne de l'application sera déplacée vers le stockage externe de l'application (Android/media/com.philkes.notallyx).
+En combinaison avec des applications de synchronisation de fichiers, cela peut être utilisé pour synchroniser les données de NotallyX entre plusieurs appareils.</t>
+  </si>
+  <si>
+    <t>Attivandolo, il database interno dell’app verrà spostato nella memoria esterna dell’app (Android/media/com.philkes.notallyx).
+Abbinandolo con un’app di sincronizzazione file potrai così sincronizzare i dati di NotallyX tra dispositivi diversi.</t>
   </si>
   <si>
     <t>启用此项，应用程序的内部数据库将被移动到应用程序的外部存储（Android / Media / Com.Philkes.notallyX）中。与文件同步应用组合，这可用于同步多个设备之间的数据。</t>
@@ -5587,17 +5597,21 @@
     <t>google_keep_help</t>
   </si>
   <si>
-    <t>In order to import your Notes from Google Keep you must download your Google Takeout ZIP file. Click Help to get more information.\n\nIf you already have a Takeout ZIP file, click Import and choose the ZIP file.</t>
-  </si>
-  <si>
-    <t>Um deine Notizen aus Google Notizen zu importieren musst du deine Google Takeout ZIP Datei herunterladen\n\nFalls du das Takeout ZIP schon hast, klicke auf Import und wähle es aus.</t>
+    <t>In order to import your Notes from Google Keep you must download your Google Takeout ZIP file. Click Help to get more information.
+If you already have a Takeout ZIP file, click Import and choose the ZIP file.</t>
+  </si>
+  <si>
+    <t>Um deine Notizen aus Google Notizen zu importieren musst du deine Google Takeout ZIP Datei herunterladen
+Falls du das Takeout ZIP schon hast, klicke auf Import und wähle es aus.</t>
   </si>
   <si>
     <t>Pour importer vos notes depuis Google Keep, vous devez télécharger votre fichier ZIP Google Takeout. Cliquez sur "Aide" pour plus d
-	information.\n\nSi vous possédez déjà un fichier ZIP Google Takeout, cliquez sur "Importer" et choisissez le fichier ZIP.</t>
-  </si>
-  <si>
-    <t>Per importare le note da Google Keep devi scaricare il tuo file ZIP di Google Takeout. Clicca su Aiuto per ulteriori informazioni.\n\nSe hai già un file ZIP di Takeout, clicca Importa e selezionalo.</t>
+	information.
+Si vous possédez déjà un fichier ZIP Google Takeout, cliquez sur "Importer" et choisissez le fichier ZIP.</t>
+  </si>
+  <si>
+    <t>Per importare le note da Google Keep devi scaricare il tuo file ZIP di Google Takeout. Clicca su Aiuto per ulteriori informazioni.
+Se hai già un file ZIP di Takeout, clicca Importa e selezionalo.</t>
   </si>
   <si>
     <t>grid</t>
@@ -5648,7 +5662,7 @@
     <t>Bildformat nicht unterstützt</t>
   </si>
   <si>
-    <t>Format d\'image non supporté</t>
+    <t>Format d'image non supporté</t>
   </si>
   <si>
     <t>Formato immagine non supportato</t>
@@ -5702,7 +5716,7 @@
     <t>Falls das Backup nicht passwortgeschützt ist, drücken Sie einfach auf Importieren, andernfalls geben Sie das richtige Passwort ein.</t>
   </si>
   <si>
-    <t>Si votre sauvegarde n\'est pas protégée par mot de passe, cliquez seulement sur "Importer une sauvegarde", sinon entrez le mot de passe correspondant.</t>
+    <t>Si votre sauvegarde n'est pas protégée par mot de passe, cliquez seulement sur "Importer une sauvegarde", sinon entrez le mot de passe correspondant.</t>
   </si>
   <si>
     <t>Se il tuo backup non è protetto da password premi semplicemente Importa, altrimenti inserisci la password corretta.</t>
@@ -5744,7 +5758,7 @@
     <t>Failed to import settings, did you choose the correct file?</t>
   </si>
   <si>
-    <t>Échec de l\'importation des paramètres, avez-vous choisi le bon fichier ?</t>
+    <t>Échec de l'importation des paramètres, avez-vous choisi le bon fichier ?</t>
   </si>
   <si>
     <t>import_settings_message</t>
@@ -5861,7 +5875,7 @@
     <t>Lege eine SD-Karte ein um Sprachnotizen aufzunehmen</t>
   </si>
   <si>
-    <t>Insérer une carte SD pour enregistrer de l\'audio</t>
+    <t>Insérer une carte SD pour enregistrer de l'audio</t>
   </si>
   <si>
     <t>Inserisci una SD card per registrare audio</t>
@@ -6077,7 +6091,7 @@
     <t>Etiqueta existe</t>
   </si>
   <si>
-    <t>L\'étiquette existe déjà</t>
+    <t>L'étiquette existe déjà</t>
   </si>
   <si>
     <t>Etichetta già esistente</t>
@@ -6098,7 +6112,7 @@
     <t>Zeige/Verberge das Label in der Navigation</t>
   </si>
   <si>
-    <t>Masquer/Afficher l\'étiquette dans le panneau de navigation</t>
+    <t>Masquer/Afficher l'étiquette dans le panneau de navigation</t>
   </si>
   <si>
     <t>Nascondi/Mostra etichetta nel pannello di navigazione</t>
@@ -6134,7 +6148,7 @@
     <t>Ist dies aktiviert, werden die Labels der Notizen in der Übersicht ausgeblendet</t>
   </si>
   <si>
-    <t>En activant cette option, les étiquettes des notes seront masquées dans la vue d\'ensemble</t>
+    <t>En activant cette option, les étiquettes des notes seront masquées dans la vue d'ensemble</t>
   </si>
   <si>
     <t>labels_hidden_in_overview_title</t>
@@ -6146,7 +6160,7 @@
     <t>Verberge Labels in Übersicht</t>
   </si>
   <si>
-    <t>Masquer les étiquettes dans la vue d\'ensemble</t>
+    <t>Masquer les étiquettes dans la vue d'ensemble</t>
   </si>
   <si>
     <t>large</t>
@@ -6347,7 +6361,7 @@
     <t>Elementos máximos para mostrar en lista</t>
   </si>
   <si>
-    <t>Nombre maximum d\'éléments à afficher pour une liste</t>
+    <t>Nombre maximum d'éléments à afficher pour une liste</t>
   </si>
   <si>
     <t>Numero massimo di elementi da mostrare nella lista</t>
@@ -6368,7 +6382,7 @@
     <t>Max. Anzahl an angezeigten Lables in der Navigation</t>
   </si>
   <si>
-    <t>Nombre maximum d\'étiquettes à afficher dans le panneau de navigation</t>
+    <t>Nombre maximum d'étiquettes à afficher dans le panneau de navigation</t>
   </si>
   <si>
     <t>Numero massimo di etichette da mostrare nel pannello di navigazione</t>
@@ -6647,22 +6661,28 @@
     <t>notes_will_be</t>
   </si>
   <si>
-    <t>Notes will be backed up to your phone’s internal storage everyday.\n\nThis may not work if you have power saving mode enabled</t>
-  </si>
-  <si>
-    <t>Notizen werden täglich auf dem internen Speicher deines Telefons gesichert.\n\nDies funktioniert möglicherweise nicht, wenn du den Energiesparmodus aktiviert hast.</t>
-  </si>
-  <si>
-    <t>Se realizará una copia de seguridad de las notas en el almacenamiento interno de su teléfono todos los días.\n\nEs posible que esto no funcione si tiene habilitado el modo de ahorro de energía</t>
-  </si>
-  <si>
-    <t>Les notes seront sauvegardées dans le stockage interne de votre téléphone tous les jours.\n\nCela peut ne pas fonctionner si le mode d\'économie d\'énergie est activé</t>
-  </si>
-  <si>
-    <t>Il backup delle note verrà salvato nella memoria interna del tuo telefono ogni giorno.\n\nCiò potrebbe non funzionare se hai la modalità di risparmio energetico attivata</t>
-  </si>
-  <si>
-    <t>笔记每天将备份到你手机的内部存储中。\n\n如果你启用了节电模式，此功能可能无法正常工作。</t>
+    <t>Notes will be backed up to your phone’s internal storage everyday.
+This may not work if you have power saving mode enabled</t>
+  </si>
+  <si>
+    <t>Notizen werden täglich auf dem internen Speicher deines Telefons gesichert.
+Dies funktioniert möglicherweise nicht, wenn du den Energiesparmodus aktiviert hast.</t>
+  </si>
+  <si>
+    <t>Se realizará una copia de seguridad de las notas en el almacenamiento interno de su teléfono todos los días.
+Es posible que esto no funcione si tiene habilitado el modo de ahorro de energía</t>
+  </si>
+  <si>
+    <t>Les notes seront sauvegardées dans le stockage interne de votre téléphone tous les jours.
+Cela peut ne pas fonctionner si le mode d'économie d'énergie est activé</t>
+  </si>
+  <si>
+    <t>Il backup delle note verrà salvato nella memoria interna del tuo telefono ogni giorno.
+Ciò potrebbe non funzionare se hai la modalità di risparmio energetico attivata</t>
+  </si>
+  <si>
+    <t>笔记每天将备份到你手机的内部存储中。
+如果你启用了节电模式，此功能可能无法正常工作。</t>
   </si>
   <si>
     <t>open_link</t>
@@ -6818,7 +6838,8 @@
     <t>In order to import your Notes from plain text files (single file or folder), click Import. Every file is imported as a separate note, the file’s name becomes the note’s title. If the text contents start with list syntax (e.g. Markdown ’- [x]’, NotallyX syntax ’[✓]’, or ’*’, ’-’) it will be converted to a List note.</t>
   </si>
   <si>
-    <t>Um deine Text-Notizen (einzele Datei oder Ordner) zu importieren, klicke Import.\n\nJede Datei wird als einzelne Notiz importiert, der Dateiname wird zum Notiz-Titel. Sollte der Textinhalt mit einer List-Syntax beginnen (z.B. Markdown ’- [x]’, NotallyX syntax ’[✓]’, or ’*’, ’-’), wird die Datei als List-Notiz importiert.</t>
+    <t>Um deine Text-Notizen (einzele Datei oder Ordner) zu importieren, klicke Import.
+Jede Datei wird als einzelne Notiz importiert, der Dateiname wird zum Notiz-Titel. Sollte der Textinhalt mit einer List-Syntax beginnen (z.B. Markdown ’- [x]’, NotallyX syntax ’[✓]’, or ’*’, ’-’), wird die Datei als List-Notiz importiert.</t>
   </si>
   <si>
     <t>Pour importer vos notes à partir de fichiers (un seul fichier ou dossier) texte bruts, cliquez sur "Importer". Chaque fichier est importé comme une note séparée, le nom du fichier devient le titre de la note. Si le contenu du texte commence par une syntaxe de liste (par exemple, Markdown ‘- [x]’, syntaxe NotallyX ‘[✓]’, ou ‘*’, ‘-’), il sera converti en une note sous forme de liste.</t>
@@ -6845,7 +6866,7 @@
     <t>Bitte gib NotallyX die Berechtigung Sprachnotizen zu erstellen. Die Aufnahmen verlassen niemals dein Gerät.</t>
   </si>
   <si>
-    <t>Veuillez accorder à NotallyX l\'autorisation d\'enregistrer de l\'audio. Les enregistrements ne quittent jamais votre appareil.</t>
+    <t>Veuillez accorder à NotallyX l'autorisation d'enregistrer de l'audio. Les enregistrements ne quittent jamais votre appareil.</t>
   </si>
   <si>
     <t>Per favore concedi a NotallyX il permesso di registrare audio. Le registrazioni non lasceranno mai il dispositivo</t>
@@ -6860,7 +6881,7 @@
     <t>Bitte erteile NotallyX die Berechtigung, Benachrichtigungen zu senden. Dies wird verwendet, um den Fortschritt anzuzeigen, wenn Vorgänge wie das Löschen von Bildern oder das Importieren von Backupen Zeit in Anspruch nehmen</t>
   </si>
   <si>
-    <t xml:space="preserve"> Veuillez accordez à NotallyX l\'autorisation d\'envoyer des notifications. Cela permet d\'afficher la progression des opérations telles que la suppression d\'images ou l\'importation de sauvegarde si elles prennent du temps.</t>
+    <t xml:space="preserve"> Veuillez accordez à NotallyX l'autorisation d'envoyer des notifications. Cela permet d'afficher la progression des opérations telles que la suppression d'images ou l'importation de sauvegarde si elles prennent du temps.</t>
   </si>
   <si>
     <t>Per favore concedi a NotallyX il permesso di inviare notifiche. Nel caso operazioni come l’eliminazione di immagini o l’importazione di backup richiedano del tempo, le notifiche vengono usate per mostrarne l’avanzamento</t>
@@ -7136,7 +7157,7 @@
     <t>Aufnahme speichern?</t>
   </si>
   <si>
-    <t>Sauvegarder l\'enregistrement ?</t>
+    <t>Sauvegarder l'enregistrement ?</t>
   </si>
   <si>
     <t>Salvare la registrazione?</t>
@@ -7151,7 +7172,7 @@
     <t>Guardar a dispositivo</t>
   </si>
   <si>
-    <t>Sauvegarder sur l\'appareil</t>
+    <t>Sauvegarder sur l'appareil</t>
   </si>
   <si>
     <t>Salva sul dispositivo</t>
@@ -7175,7 +7196,7 @@
     <t>Guardada en dispositivo</t>
   </si>
   <si>
-    <t>Sauvegardé sur l\'appareil</t>
+    <t>Sauvegardé sur l'appareil</t>
   </si>
   <si>
     <t>Salvata sul dispositivo</t>
@@ -7442,16 +7463,20 @@
     <t>something_went_wrong_audio</t>
   </si>
   <si>
-    <t>Something went wrong. The audio recording may have been moved or deleted.\n\nError : (%1$d, %2$d)</t>
-  </si>
-  <si>
-    <t>Etwas lief schief. Die Sprachnotiz wurde eventuell verschoben oder gelöscht.\n\nFehler : (%1$d, %2$d)</t>
-  </si>
-  <si>
-    <t>Une erreur est survenue. l\'enregistrement audio a peut-être été déplacé ou supprimé.\n\nErreur : (%1$d, %2$d)</t>
-  </si>
-  <si>
-    <t>Qualcosa è andato storto. La registrazione audio potrebbe essere stata spostata o rimossa.\n\nErrore : (%1$d, %2$d)</t>
+    <t>Something went wrong. The audio recording may have been moved or deleted.
+Error : (%1$d, %2$d)</t>
+  </si>
+  <si>
+    <t>Etwas lief schief. Die Sprachnotiz wurde eventuell verschoben oder gelöscht.
+Fehler : (%1$d, %2$d)</t>
+  </si>
+  <si>
+    <t>Une erreur est survenue. l'enregistrement audio a peut-être été déplacé ou supprimé.
+Erreur : (%1$d, %2$d)</t>
+  </si>
+  <si>
+    <t>Qualcosa è andato storto. La registrazione audio potrebbe essere stata spostata o rimossa.
+Errore : (%1$d, %2$d)</t>
   </si>
   <si>
     <t>sort_direction</t>
@@ -7556,7 +7581,7 @@
     <t>Klick für mehr Optionen</t>
   </si>
   <si>
-    <t>Toucher pour afficher plus d\'options</t>
+    <t>Toucher pour afficher plus d'options</t>
   </si>
   <si>
     <t>Tocca per ulteriori opzioni</t>
@@ -7658,7 +7683,7 @@
     <t>Um Sprachnotizen zu erstellen, braucht NotallyX Zugriff auf dein Mikrofon. Klicke Einstellunge &gt; Berechtigungen und aktiviere Mikrofon</t>
   </si>
   <si>
-    <t>Pour enregistrer de l\'audio, autorisez NotallyX à accéder à votre microphone. Cliquez sur Paramètres &gt; Autorisations et activez le microphone.</t>
+    <t>Pour enregistrer de l'audio, autorisez NotallyX à accéder à votre microphone. Cliquez sur Paramètres &gt; Autorisations et activez le microphone.</t>
   </si>
   <si>
     <t>Per registrare audio, consenti a NotallyX di accedere al tuo microfono. Vai su Impostazioni &gt; Permessi e attiva il microfono</t>

</xml_diff>